<commit_message>
stepper page login data chnages
</commit_message>
<xml_diff>
--- a/src/test/resources/Excels/NOVO_testcases_masterexcel.xlsx
+++ b/src/test/resources/Excels/NOVO_testcases_masterexcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlakkamraju\eclipse-workspace\Novo_Hybrid_FrameWork\src\test\resources\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlakkamraju\eclipse-workspace\Novo_Hybrid_framework_code\src\test\resources\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -169,9 +169,6 @@
     <t>SkillLevel</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Software Quality Assurance</t>
   </si>
   <si>
@@ -191,6 +188,15 @@
   </si>
   <si>
     <t>Apache JMeter</t>
+  </si>
+  <si>
+    <t>automationtest@pixentia.com</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -716,7 +722,7 @@
         <v>40</v>
       </c>
       <c r="N1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -730,7 +736,7 @@
         <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
@@ -774,7 +780,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -822,32 +828,35 @@
       <c r="A2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>53</v>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
         <v>49</v>
       </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>